<commit_message>
fix: fix bug, add some docs
</commit_message>
<xml_diff>
--- a/autoregfile/examples/test/test_regfile.xlsx
+++ b/autoregfile/examples/test/test_regfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\ICProject\github_clone\auto_scripts_demo\autoregfile\examples\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CA5C0C-571B-491E-A141-E4BF187474C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54C495D-DAF8-4AD7-A560-61F92A4D2D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="0" windowWidth="21840" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
   <si>
     <t>parameter</t>
   </si>
@@ -227,25 +227,10 @@
     <t>写1置位寄存器</t>
   </si>
   <si>
-    <t>BIT0</t>
-  </si>
-  <si>
-    <t>写1置位的位字段</t>
-  </si>
-  <si>
-    <t>软件写1置位此位</t>
-  </si>
-  <si>
     <t>LOCK_TEST_REG</t>
   </si>
   <si>
     <t>0x14</t>
-  </si>
-  <si>
-    <t>0x12345678</t>
-  </si>
-  <si>
-    <t>锁测试寄存器</t>
   </si>
   <si>
     <t>LOCKED_FIELD</t>
@@ -783,7 +768,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -816,7 +801,7 @@
         <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>20</v>
@@ -954,7 +939,7 @@
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H7" t="s">
         <v>47</v>
@@ -983,7 +968,7 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
         <v>47</v>
@@ -1043,13 +1028,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -1058,7 +1043,7 @@
         <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J11" t="s">
         <v>65</v>
@@ -1066,13 +1051,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
         <v>27</v>
@@ -1081,58 +1066,26 @@
         <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" t="s">
-        <v>69</v>
-      </c>
-      <c r="K13" t="s">
-        <v>70</v>
-      </c>
-    </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
         <v>27</v>
@@ -1141,24 +1094,24 @@
         <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
         <v>27</v>
@@ -1167,16 +1120,16 @@
         <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="K16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="M16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>